<commit_message>
Curtis - Added LCD_Display.vhd
git-svn-id: https://cjfileserver/svn/cachemoney@35 bcaa0796-ab92-4845-b78f-7ce167744df0
</commit_message>
<xml_diff>
--- a/trunk/lcd_info/lcd_display.xlsx
+++ b/trunk/lcd_info/lcd_display.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>RS</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>8bit character code</t>
+  </si>
+  <si>
+    <t>Max clock for lcd</t>
+  </si>
+  <si>
+    <t>25.641 khz</t>
   </si>
 </sst>
 </file>
@@ -111,8 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,16 +607,24 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>